<commit_message>
implemented run creation stump
</commit_message>
<xml_diff>
--- a/templates/v1.xlsx
+++ b/templates/v1.xlsx
@@ -156,11 +156,11 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -803,8 +803,8 @@
   </sheetPr>
   <dimension ref="A9:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +856,6 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12">
-        <f t="shared" ref="H12:H23" si="0">A12</f>
         <v>1</v>
       </c>
     </row>
@@ -866,7 +865,6 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -876,7 +874,6 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -886,7 +883,6 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -896,7 +892,6 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -906,7 +901,6 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -916,7 +910,6 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -926,7 +919,6 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -936,7 +928,6 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -946,7 +937,6 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -956,7 +946,6 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
@@ -966,7 +955,6 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -996,10 +984,10 @@
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="9"/>
+      <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
@@ -1009,8 +997,8 @@
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
@@ -1019,10 +1007,10 @@
       <c r="D29" s="5"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="8"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>

</xml_diff>